<commit_message>
Implement Function to Update Quantity
Implement Function to Update Quantity
Complete Event Loop
</commit_message>
<xml_diff>
--- a/Asset Management/assets.xlsx
+++ b/Asset Management/assets.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ACF2575-EC9D-4B6D-8D37-F564E0E60499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{755AA496-DB5E-41E8-8A13-F618875B0655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,15 +30,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Asset Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Asset Label</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Söhne"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +398,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>